<commit_message>
changes as part of testing
</commit_message>
<xml_diff>
--- a/3EAH-02 DRR try (1).xlsx
+++ b/3EAH-02 DRR try (1).xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poojitha.reddy.soma\Git_practice\python-trainings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39550239-92B3-420F-AFF5-9316D825A2E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Cut-In Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="vamsi" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="difference" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Data Cut-In Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="vamsi" sheetId="2" r:id="rId2"/>
+    <sheet name="difference" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Data Cut-In Summary'!$A$1:$U$62</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Data Cut-In Summary'!$A$1:$U$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Cut-In Summary'!$A$1:$U$62</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="526">
   <si>
     <t>DPU_ID</t>
   </si>
@@ -1602,27 +1608,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1638,16 +1643,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1671,7 +1675,15 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1995,117 +2007,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="3" width="19.42578125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="3" width="12.28515625"/>
-    <col customWidth="1" hidden="1" max="3" min="3" style="3" width="23.85546875"/>
-    <col customWidth="1" hidden="1" max="4" min="4" style="3" width="12.7109375"/>
-    <col customWidth="1" hidden="1" max="5" min="5" style="3" width="16.42578125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="3" width="16.5703125"/>
-    <col customWidth="1" hidden="1" max="7" min="7" style="3" width="18"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="3" width="34.140625"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="3" width="16.7109375"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="3" width="19.42578125"/>
-    <col customWidth="1" hidden="1" max="11" min="11" style="3" width="18.7109375"/>
-    <col customWidth="1" hidden="1" max="12" min="12" style="3" width="15"/>
-    <col customWidth="1" hidden="1" max="13" min="13" style="3" width="11.7109375"/>
-    <col customWidth="1" hidden="1" max="14" min="14" style="3" width="15.42578125"/>
-    <col customWidth="1" hidden="1" max="15" min="15" style="3" width="20.28515625"/>
-    <col customWidth="1" hidden="1" max="16" min="16" style="3" width="18.28515625"/>
-    <col customWidth="1" hidden="1" max="17" min="17" style="3" width="55.28515625"/>
-    <col customWidth="1" hidden="1" max="18" min="18" style="3" width="13.5703125"/>
-    <col customWidth="1" hidden="1" max="19" min="19" style="3" width="22.140625"/>
-    <col customWidth="1" hidden="1" max="20" min="20" style="3" width="16.140625"/>
-    <col customWidth="1" hidden="1" max="21" min="21" style="3" width="28.5703125"/>
-    <col customWidth="1" max="22" min="22" style="3" width="9.140625"/>
-    <col customWidth="1" max="16384" min="23" style="3" width="9.140625"/>
+    <col min="1" max="1" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="2" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="55.28515625" style="2" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" style="2" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="28.5703125" style="2" hidden="1" customWidth="1"/>
+    <col min="22" max="23" width="9.140625" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>-1</v>
       </c>
       <c r="D2" t="s">
@@ -2157,14 +2165,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>-1</v>
       </c>
       <c r="D3" t="s">
@@ -2219,11 +2227,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
@@ -2275,14 +2283,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>-1</v>
       </c>
       <c r="D5" t="s">
@@ -2337,14 +2345,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>-1</v>
       </c>
       <c r="D6" t="s">
@@ -2396,14 +2404,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>-1</v>
       </c>
       <c r="D7" t="s">
@@ -2458,14 +2466,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>-1</v>
       </c>
       <c r="D8" t="s">
@@ -2520,14 +2528,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>95</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>-1</v>
       </c>
       <c r="D9" t="s">
@@ -2582,11 +2590,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>104</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>2</v>
       </c>
       <c r="F10" t="s">
@@ -2638,14 +2646,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>-1</v>
       </c>
       <c r="D11" t="s">
@@ -2700,11 +2708,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>122</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>2</v>
       </c>
       <c r="F12" t="s">
@@ -2756,14 +2764,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>131</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>-1</v>
       </c>
       <c r="D13" t="s">
@@ -2818,11 +2826,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>140</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>4</v>
       </c>
       <c r="F14" t="s">
@@ -2874,14 +2882,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>150</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>-1</v>
       </c>
       <c r="D15" t="s">
@@ -2936,11 +2944,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>159</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>4</v>
       </c>
       <c r="F16" t="s">
@@ -2992,14 +3000,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>159</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>4</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>-1</v>
       </c>
       <c r="D17" t="s">
@@ -3051,11 +3059,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>172</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>3</v>
       </c>
       <c r="F18" t="s">
@@ -3107,14 +3115,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>181</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>4</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>-1</v>
       </c>
       <c r="D19" t="s">
@@ -3169,14 +3177,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>190</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>3</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>-1</v>
       </c>
       <c r="D20" t="s">
@@ -3231,14 +3239,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>199</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>2</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>-1</v>
       </c>
       <c r="D21" t="s">
@@ -3290,14 +3298,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>208</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>4</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>-1</v>
       </c>
       <c r="D22" t="s">
@@ -3352,14 +3360,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>217</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>2</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>-1</v>
       </c>
       <c r="D23" t="s">
@@ -3414,11 +3422,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>226</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>4</v>
       </c>
       <c r="F24" t="s">
@@ -3470,14 +3478,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>235</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>-1</v>
       </c>
       <c r="D25" t="s">
@@ -3493,11 +3501,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>238</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
@@ -3549,14 +3557,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>247</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>2</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>-1</v>
       </c>
       <c r="D27" t="s">
@@ -3572,11 +3580,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>250</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>2</v>
       </c>
       <c r="F28" t="s">
@@ -3628,14 +3636,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>259</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
         <v>-1</v>
       </c>
       <c r="D29" t="s">
@@ -3651,11 +3659,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>262</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>1</v>
       </c>
       <c r="F30" t="s">
@@ -3698,14 +3706,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>262</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>2</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31">
         <v>-1</v>
       </c>
       <c r="D31" t="s">
@@ -3760,11 +3768,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>262</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>3</v>
       </c>
       <c r="F32" t="s">
@@ -3816,14 +3824,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>287</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>2</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33">
         <v>-1</v>
       </c>
       <c r="D33" t="s">
@@ -3878,11 +3886,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>296</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>3</v>
       </c>
       <c r="F34" t="s">
@@ -3934,14 +3942,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>262</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>4</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35">
         <v>-1</v>
       </c>
       <c r="D35" t="s">
@@ -3957,14 +3965,14 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>307</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>2</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36">
         <v>-1</v>
       </c>
       <c r="D36" t="s">
@@ -4019,11 +4027,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>316</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>2</v>
       </c>
       <c r="F37" t="s">
@@ -4075,14 +4083,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>325</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>3</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38">
         <v>-1</v>
       </c>
       <c r="D38" t="s">
@@ -4137,14 +4145,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>334</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>4</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39">
         <v>-1</v>
       </c>
       <c r="D39" t="s">
@@ -4199,14 +4207,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>86</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>2</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40">
         <v>-1</v>
       </c>
       <c r="D40" t="s">
@@ -4222,14 +4230,14 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>1</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41">
         <v>-1</v>
       </c>
       <c r="D41" t="s">
@@ -4245,11 +4253,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>347</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>2</v>
       </c>
       <c r="F42" t="s">
@@ -4301,14 +4309,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>356</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>1</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43">
         <v>-1</v>
       </c>
       <c r="D43" t="s">
@@ -4363,11 +4371,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:21">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>365</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>3</v>
       </c>
       <c r="F44" t="s">
@@ -4419,14 +4427,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>374</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>1</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45">
         <v>-1</v>
       </c>
       <c r="D45" t="s">
@@ -4481,11 +4489,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>383</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>2</v>
       </c>
       <c r="F46" t="s">
@@ -4537,14 +4545,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>392</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>2</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47">
         <v>-1</v>
       </c>
       <c r="D47" t="s">
@@ -4599,14 +4607,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>392</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>2</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48">
         <v>-1</v>
       </c>
       <c r="D48" t="s">
@@ -4661,11 +4669,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:21">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>402</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>1</v>
       </c>
       <c r="F49" t="s">
@@ -4717,14 +4725,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:21">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>411</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>3</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50">
         <v>-1</v>
       </c>
       <c r="D50" t="s">
@@ -4779,11 +4787,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:21">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>420</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>2</v>
       </c>
       <c r="F51" t="s">
@@ -4835,14 +4843,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:21">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>428</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>1</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52">
         <v>-1</v>
       </c>
       <c r="D52" t="s">
@@ -4897,11 +4905,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:21">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>437</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>2</v>
       </c>
       <c r="F53" t="s">
@@ -4953,14 +4961,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:21">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>446</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>3</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54">
         <v>-1</v>
       </c>
       <c r="D54" t="s">
@@ -5015,11 +5023,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:21">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>150</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55">
         <v>4</v>
       </c>
       <c r="F55" t="s">
@@ -5071,14 +5079,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:21">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>464</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56">
         <v>3</v>
       </c>
-      <c r="C56" t="n">
+      <c r="C56">
         <v>-1</v>
       </c>
       <c r="D56" t="s">
@@ -5133,11 +5141,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:21">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>473</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>4</v>
       </c>
       <c r="F57" t="s">
@@ -5189,14 +5197,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:21">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>482</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>4</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58">
         <v>-1</v>
       </c>
       <c r="D58" t="s">
@@ -5251,11 +5259,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:21">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>491</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59">
         <v>3</v>
       </c>
       <c r="F59" t="s">
@@ -5304,14 +5312,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:21">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>500</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60">
         <v>2</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60">
         <v>-1</v>
       </c>
       <c r="D60" t="s">
@@ -5366,11 +5374,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:21">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>509</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61">
         <v>2</v>
       </c>
       <c r="F61" t="s">
@@ -5422,14 +5430,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:21">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>517</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62">
         <v>1</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62">
         <v>-1</v>
       </c>
       <c r="D62" t="s">
@@ -5485,607 +5493,597 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U62"/>
+  <autoFilter ref="A1:U62" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="F1:F46 F48:F1048576">
-    <cfRule dxfId="0" priority="2" type="duplicateValues"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47">
-    <cfRule dxfId="0" priority="1" type="duplicateValues"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="3" width="16.7109375"/>
+    <col min="1" max="1" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="1:1"/>
-    <row r="26" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:1"/>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="1:1"/>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="35" spans="1:1"/>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:1"/>
-    <row r="41" spans="1:1"/>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>520</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>229</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>